<commit_message>
touch-ups for 4-th test
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetBanking/testData/NewCustomerData.xlsx
+++ b/src/test/java/com/inetBanking/testData/NewCustomerData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -118,25 +117,25 @@
     <t>111111</t>
   </si>
   <si>
+    <t>6035154545</t>
+  </si>
+  <si>
+    <t>1231230088</t>
+  </si>
+  <si>
+    <t>1177777777</t>
+  </si>
+  <si>
+    <t>passw1</t>
+  </si>
+  <si>
+    <t>anypass</t>
+  </si>
+  <si>
+    <t>p33311</t>
+  </si>
+  <si>
     <t>343434</t>
-  </si>
-  <si>
-    <t>6035154545</t>
-  </si>
-  <si>
-    <t>1231230088</t>
-  </si>
-  <si>
-    <t>1177777777</t>
-  </si>
-  <si>
-    <t>passw1</t>
-  </si>
-  <si>
-    <t>anypass</t>
-  </si>
-  <si>
-    <t>p33311</t>
   </si>
 </sst>
 </file>
@@ -511,7 +510,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,10 +588,10 @@
         <v>30</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -624,10 +623,10 @@
         <v>31</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -656,13 +655,13 @@
         <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>